<commit_message>
Official submission of BlackJack V.1.0
See BlackJack Final Submission and known bugs.docx for more details.
</commit_message>
<xml_diff>
--- a/GUI Design.xlsx
+++ b/GUI Design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Name: J</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>BET_TEXT_FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -555,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
@@ -644,6 +647,11 @@
       </c>
       <c r="E5" s="9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>